<commit_message>
updated from ROG laptop
ST paper corrections and tirell study data
</commit_message>
<xml_diff>
--- a/R/Included/New_Scoring.xlsx
+++ b/R/Included/New_Scoring.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LPersad\Documents\GitHub\Systematic_lit_review\R\Included\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrf_g\Documents\GitHub\Systematic_lit_review\R\Included\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D167625-969E-4314-955D-FA8791D6A586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17400"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Torque-Force" sheetId="2" r:id="rId1"/>
@@ -21,12 +22,25 @@
     <sheet name="ST" sheetId="7" r:id="rId7"/>
     <sheet name="Scoring flowchart" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="114">
   <si>
     <t>MRI, CSA x slice interval</t>
   </si>
@@ -293,13 +307,89 @@
   </si>
   <si>
     <t>Tendon force</t>
+  </si>
+  <si>
+    <t>[4162]</t>
+  </si>
+  <si>
+    <t>[4127]</t>
+  </si>
+  <si>
+    <t>[2995]</t>
+  </si>
+  <si>
+    <t>[2833]</t>
+  </si>
+  <si>
+    <t>[2651]</t>
+  </si>
+  <si>
+    <t>[4196]</t>
+  </si>
+  <si>
+    <t>[4040]</t>
+  </si>
+  <si>
+    <t>[2820]</t>
+  </si>
+  <si>
+    <t>[2672]</t>
+  </si>
+  <si>
+    <t>[4050]</t>
+  </si>
+  <si>
+    <t>[4204]</t>
+  </si>
+  <si>
+    <t>[2899]</t>
+  </si>
+  <si>
+    <t>[4135 2821 2938 2745]</t>
+  </si>
+  <si>
+    <t>[4128 2677 3042]</t>
+  </si>
+  <si>
+    <t>[2837 4106]</t>
+  </si>
+  <si>
+    <t>[2680 2664 2653 2649 2648]</t>
+  </si>
+  <si>
+    <t>[2677 2646]</t>
+  </si>
+  <si>
+    <t>[4070 4205]</t>
+  </si>
+  <si>
+    <t>CovidenceID</t>
+  </si>
+  <si>
+    <t>OLD_SCORE</t>
+  </si>
+  <si>
+    <t>[4162 4135 4128 2995 2837 2833 2821 2680 2677 2664 2653 2651 2649 2648
+ 2646 4196 4106 4070 4040 2938 2745 2672 4205 4050]</t>
+  </si>
+  <si>
+    <t>[2995 2677]</t>
+  </si>
+  <si>
+    <t>[2820 2899]</t>
+  </si>
+  <si>
+    <t>[3042]</t>
+  </si>
+  <si>
+    <t>StudyID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,6 +402,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -349,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -357,7 +454,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,6 +463,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,189 +767,311 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="103.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C4" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
       <c r="B6">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
       <c r="B7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
       <c r="B8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
       <c r="B9">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="B12">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
       <c r="B13">
+        <v>18</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="7">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>34</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C16" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>35</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
       <c r="B18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
       <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="7">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
       <c r="B20">
         <v>4</v>
       </c>
-    </row>
+      <c r="C20" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,7 +1173,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1020,11 +1241,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,7 +1331,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1135,7 +1356,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1143,7 +1364,7 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1159,7 +1380,7 @@
         <v>45</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1168,80 +1389,102 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="3" max="3" width="106.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
       <c r="B5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8">
         <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1250,7 +1493,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1308,7 +1551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A4:R30"/>
   <sheetViews>
     <sheetView topLeftCell="J13" workbookViewId="0">
@@ -1334,7 +1577,7 @@
     <col min="18" max="18" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>62</v>
       </c>
@@ -1345,7 +1588,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1365,7 +1608,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1384,14 +1627,14 @@
       <c r="H6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1410,12 +1653,12 @@
       <c r="H8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -1434,50 +1677,48 @@
       <c r="H10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I14" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="4" t="s">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
     </row>
     <row r="19" spans="12:18" ht="60" x14ac:dyDescent="0.25">
       <c r="L19" s="2" t="s">

</xml_diff>